<commit_message>
added functions for getting email list, grades and usernames
</commit_message>
<xml_diff>
--- a/email_test_scores.xlsx
+++ b/email_test_scores.xlsx
@@ -155,10 +155,10 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
   </cols>
@@ -184,7 +184,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added a final function that sends the mail
</commit_message>
<xml_diff>
--- a/email_test_scores.xlsx
+++ b/email_test_scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">email1@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">royalty0013@gmail.com</t>
+    <t xml:space="preserve">njklnlk;@hknl.comkl</t>
   </si>
   <si>
     <t xml:space="preserve">tdunia@ymail.com</t>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">ejdunia@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
   </si>
 </sst>
 </file>
@@ -152,13 +155,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
   </cols>
@@ -211,13 +214,17 @@
         <v>90</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="email1@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="royalty0013@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="tdunia@ymail.com"/>
-    <hyperlink ref="A5" r:id="rId4" display="prhataz@gmail.com"/>
-    <hyperlink ref="A6" r:id="rId5" display="ejdunia@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="tdunia@ymail.com"/>
+    <hyperlink ref="A5" r:id="rId3" display="prhataz@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId4" display="ejdunia@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>